<commit_message>
adding id to properties files
</commit_message>
<xml_diff>
--- a/datasheets/empty_model.xlsx
+++ b/datasheets/empty_model.xlsx
@@ -998,7 +998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C1:CR1"/>
+  <dimension ref="A1:CR1"/>
   <sheetViews>
     <sheetView topLeftCell="CA1" workbookViewId="0">
       <selection activeCell="CA2" sqref="A2:XFD2"/>
@@ -1007,464 +1007,474 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cohortDataTypes|id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>cohortDataTypes|label</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>cohortDataTypes|id</t>
+          <t>cohortDesign|id</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>cohortDataTypes|label</t>
+          <t>cohortDesign|label</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>cohortDesign|id</t>
+          <t>cohortSize</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>cohortDesign|label</t>
+          <t>cohortType</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>cohortSize</t>
+          <t>collectionEvents|eventAgeRange|availability</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>cohortType</t>
+          <t>collectionEvents|eventAgeRange|availabilityCount</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventAgeRange|availability</t>
+          <t>collectionEvents|eventAgeRange|distribution</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventAgeRange|availabilityCount</t>
+          <t>collectionEvents|eventDataTypes|availability</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventAgeRange|distribution</t>
+          <t>collectionEvents|eventDataTypes|availabilityCount</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventDataTypes|availability</t>
+          <t>collectionEvents|eventDataTypes|distribution</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventDataTypes|availabilityCount</t>
+          <t>collectionEvents|eventDiseases|availability</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventDataTypes|distribution</t>
+          <t>collectionEvents|eventDiseases|availabilityCount</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventDiseases|availability</t>
+          <t>collectionEvents|eventDiseases|distribution</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventDiseases|availabilityCount</t>
+          <t>collectionEvents|eventEthnicities|availability</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventDiseases|distribution</t>
+          <t>collectionEvents|eventEthnicities|availabilityCount</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventEthnicities|availability</t>
+          <t>collectionEvents|eventEthnicities|distribution</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventEthnicities|availabilityCount</t>
+          <t>collectionEvents|eventGenders|availability</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventEthnicities|distribution</t>
+          <t>collectionEvents|eventGenders|availabilityCount</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventGenders|availability</t>
+          <t>collectionEvents|eventGenders|distribution</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventGenders|availabilityCount</t>
+          <t>collectionEvents|eventLocations|availability</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventGenders|distribution</t>
+          <t>collectionEvents|eventLocations|availabilityCount</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventLocations|availability</t>
+          <t>collectionEvents|eventLocations|distribution</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventLocations|availabilityCount</t>
+          <t>collectionEvents|eventPhenotypes|availability</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventLocations|distribution</t>
+          <t>collectionEvents|eventPhenotypes|availabilityCount</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventPhenotypes|availability</t>
+          <t>collectionEvents|eventPhenotypes|distribution</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventPhenotypes|availabilityCount</t>
+          <t>collectionEvents|eventTimeline|availability</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventPhenotypes|distribution</t>
+          <t>collectionEvents|eventTimeline|availabilityCount</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventTimeline|availability</t>
+          <t>collectionEvents|eventTimeline|distribution</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventTimeline|availabilityCount</t>
+          <t>exclusionCriteria|ageRange</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>collectionEvents|eventTimeline|distribution</t>
+          <t>exclusionCriteria|ageRange|end|iso8601duration</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|ageRange</t>
+          <t>exclusionCriteria|ageRange|start|iso8601duration</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|ageRange|end|iso8601duration</t>
+          <t>exclusionCriteria|diseaseConditions|ageOfOnset</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|ageRange|start|iso8601duration</t>
+          <t>exclusionCriteria|diseaseConditions|diseaseCode|id</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|ageOfOnset</t>
+          <t>exclusionCriteria|diseaseConditions|diseaseCode|label</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|diseaseCode|id</t>
+          <t>exclusionCriteria|diseaseConditions|familyHistory</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|diseaseCode|label</t>
+          <t>exclusionCriteria|diseaseConditions|notes</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|familyHistory</t>
+          <t>exclusionCriteria|diseaseConditions|severity|id</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|notes</t>
+          <t>exclusionCriteria|diseaseConditions|severity|label</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|severity|id</t>
+          <t>exclusionCriteria|diseaseConditions|stage|id</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|severity|label</t>
+          <t>exclusionCriteria|diseaseConditions|stage|label</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|stage|id</t>
+          <t>exclusionCriteria|ethnicities|id</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|diseaseConditions|stage|label</t>
+          <t>exclusionCriteria|ethnicities|label</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|ethnicities|id</t>
+          <t>exclusionCriteria|genders|id</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|ethnicities|label</t>
+          <t>exclusionCriteria|genders|label</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|genders|id</t>
+          <t>exclusionCriteria|locations|id</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|genders|label</t>
+          <t>exclusionCriteria|locations|label</t>
         </is>
       </c>
       <c r="AW1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|locations|id</t>
+          <t>exclusionCriteria|phenotypicConditions|evidence|evidenceCode</t>
         </is>
       </c>
       <c r="AX1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|locations|label</t>
+          <t>exclusionCriteria|phenotypicConditions|evidence|reference</t>
         </is>
       </c>
       <c r="AY1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|evidence|evidenceCode</t>
+          <t>exclusionCriteria|phenotypicConditions|excluded</t>
         </is>
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|evidence|reference</t>
+          <t>exclusionCriteria|phenotypicConditions|featureType|id</t>
         </is>
       </c>
       <c r="BA1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|excluded</t>
+          <t>exclusionCriteria|phenotypicConditions|featureType|label</t>
         </is>
       </c>
       <c r="BB1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|featureType|id</t>
+          <t>exclusionCriteria|phenotypicConditions|modifiers</t>
         </is>
       </c>
       <c r="BC1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|featureType|label</t>
+          <t>exclusionCriteria|phenotypicConditions|notes</t>
         </is>
       </c>
       <c r="BD1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|modifiers</t>
+          <t>exclusionCriteria|phenotypicConditions|onset</t>
         </is>
       </c>
       <c r="BE1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|notes</t>
+          <t>exclusionCriteria|phenotypicConditions|resolution</t>
         </is>
       </c>
       <c r="BF1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|onset</t>
+          <t>exclusionCriteria|phenotypicConditions|severity|id</t>
         </is>
       </c>
       <c r="BG1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|resolution</t>
+          <t>exclusionCriteria|phenotypicConditions|severity|label</t>
         </is>
       </c>
       <c r="BH1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|severity|id</t>
+          <t>exclusionCriteria|type|availability</t>
         </is>
       </c>
       <c r="BI1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|phenotypicConditions|severity|label</t>
+          <t>exclusionCriteria|type|availabilityCount</t>
         </is>
       </c>
       <c r="BJ1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|type|availability</t>
+          <t>id</t>
         </is>
       </c>
       <c r="BK1" t="inlineStr">
         <is>
-          <t>exclusionCriteria|type|availabilityCount</t>
+          <t>inclusionCriteria|ageRange</t>
         </is>
       </c>
       <c r="BL1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>inclusionCriteria|ageRange|end|iso8601duration</t>
         </is>
       </c>
       <c r="BM1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|ageRange</t>
+          <t>inclusionCriteria|ageRange|start|iso8601duration</t>
         </is>
       </c>
       <c r="BN1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|ageRange|end|iso8601duration</t>
+          <t>inclusionCriteria|diseaseConditions|ageOfOnset</t>
         </is>
       </c>
       <c r="BO1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|ageRange|start|iso8601duration</t>
+          <t>inclusionCriteria|diseaseConditions|diseaseCode|id</t>
         </is>
       </c>
       <c r="BP1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|ageOfOnset</t>
+          <t>inclusionCriteria|diseaseConditions|diseaseCode|label</t>
         </is>
       </c>
       <c r="BQ1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|diseaseCode|id</t>
+          <t>inclusionCriteria|diseaseConditions|familyHistory</t>
         </is>
       </c>
       <c r="BR1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|diseaseCode|label</t>
+          <t>inclusionCriteria|diseaseConditions|notes</t>
         </is>
       </c>
       <c r="BS1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|familyHistory</t>
+          <t>inclusionCriteria|diseaseConditions|severity|id</t>
         </is>
       </c>
       <c r="BT1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|notes</t>
+          <t>inclusionCriteria|diseaseConditions|severity|label</t>
         </is>
       </c>
       <c r="BU1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|severity|id</t>
+          <t>inclusionCriteria|diseaseConditions|stage|id</t>
         </is>
       </c>
       <c r="BV1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|severity|label</t>
+          <t>inclusionCriteria|diseaseConditions|stage|label</t>
         </is>
       </c>
       <c r="BW1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|stage|id</t>
+          <t>inclusionCriteria|ethnicities|id</t>
         </is>
       </c>
       <c r="BX1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|diseaseConditions|stage|label</t>
+          <t>inclusionCriteria|ethnicities|label</t>
         </is>
       </c>
       <c r="BY1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|ethnicities|id</t>
+          <t>inclusionCriteria|genders|id</t>
         </is>
       </c>
       <c r="BZ1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|ethnicities|label</t>
+          <t>inclusionCriteria|genders|label</t>
         </is>
       </c>
       <c r="CA1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|genders|id</t>
+          <t>inclusionCriteria|locations|id</t>
         </is>
       </c>
       <c r="CB1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|genders|label</t>
+          <t>inclusionCriteria|locations|label</t>
         </is>
       </c>
       <c r="CC1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|locations|id</t>
+          <t>inclusionCriteria|phenotypicConditions|evidence|evidenceCode</t>
         </is>
       </c>
       <c r="CD1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|locations|label</t>
+          <t>inclusionCriteria|phenotypicConditions|evidence|reference</t>
         </is>
       </c>
       <c r="CE1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|evidence|evidenceCode</t>
+          <t>inclusionCriteria|phenotypicConditions|excluded</t>
         </is>
       </c>
       <c r="CF1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|evidence|reference</t>
+          <t>inclusionCriteria|phenotypicConditions|featureType|id</t>
         </is>
       </c>
       <c r="CG1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|excluded</t>
+          <t>inclusionCriteria|phenotypicConditions|featureType|label</t>
         </is>
       </c>
       <c r="CH1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|featureType|id</t>
+          <t>inclusionCriteria|phenotypicConditions|modifiers</t>
         </is>
       </c>
       <c r="CI1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|featureType|label</t>
+          <t>inclusionCriteria|phenotypicConditions|notes</t>
         </is>
       </c>
       <c r="CJ1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|modifiers</t>
+          <t>inclusionCriteria|phenotypicConditions|onset</t>
         </is>
       </c>
       <c r="CK1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|notes</t>
+          <t>inclusionCriteria|phenotypicConditions|resolution</t>
         </is>
       </c>
       <c r="CL1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|onset</t>
+          <t>inclusionCriteria|phenotypicConditions|severity|id</t>
         </is>
       </c>
       <c r="CM1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|resolution</t>
+          <t>inclusionCriteria|phenotypicConditions|severity|label</t>
         </is>
       </c>
       <c r="CN1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|severity|id</t>
+          <t>inclusionCriteria|type|availability</t>
         </is>
       </c>
       <c r="CO1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|phenotypicConditions|severity|label</t>
+          <t>inclusionCriteria|type|availabilityCount</t>
         </is>
       </c>
       <c r="CP1" t="inlineStr">
         <is>
-          <t>inclusionCriteria|type|availability</t>
+          <t>name</t>
         </is>
       </c>
       <c r="CQ1" t="inlineStr">

</xml_diff>

<commit_message>
multi conversion to csv added
</commit_message>
<xml_diff>
--- a/datasheets/empty_model.xlsx
+++ b/datasheets/empty_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oriol/Desktop/beacon-ri-tools-v2/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB58E01-BCB0-E742-883E-E4EE7C951F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EE5DEA-442B-8048-9796-101E2BC773E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="analyses" sheetId="1" r:id="rId1"/>
@@ -1561,9 +1561,6 @@
     <t>runDate</t>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
     <t>female</t>
   </si>
   <si>
@@ -1601,6 +1598,9 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>male,female</t>
   </si>
 </sst>
 </file>
@@ -2000,35 +2000,35 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -2330,35 +2330,35 @@
     </row>
     <row r="2" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="CG2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="CG3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="4" spans="1:94" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="CG4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -2731,7 +2731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:GJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+    <sheetView topLeftCell="BH1" workbookViewId="0">
       <selection activeCell="BV3" sqref="BV3"/>
     </sheetView>
   </sheetViews>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="2" spans="1:192" x14ac:dyDescent="0.2">
       <c r="AY2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -3329,8 +3329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:EH4"/>
   <sheetViews>
-    <sheetView topLeftCell="DJ1" workbookViewId="0">
-      <selection activeCell="DX5" sqref="DX5"/>
+    <sheetView tabSelected="1" topLeftCell="DJ1" workbookViewId="0">
+      <selection activeCell="DX3" sqref="DX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3756,7 +3756,7 @@
         <v>499</v>
       </c>
       <c r="DX2" t="s">
-        <v>511</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:138" x14ac:dyDescent="0.2">
@@ -3764,7 +3764,7 @@
         <v>500</v>
       </c>
       <c r="DX3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="4" spans="1:138" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
         <v>501</v>
       </c>
       <c r="DX4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>